<commit_message>
Enhance: add progress bars for scheduling and output, remove debug prints, improve soft constraint reporting, update docs and requirements
</commit_message>
<xml_diff>
--- a/solution_v3/data/courses.xlsx
+++ b/solution_v3/data/courses.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MATH101</t>
+          <t>LEM</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -497,12 +497,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1DA</t>
+          <t>ALGAN</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Prof_A</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -512,7 +512,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PHYS101</t>
+          <t>LEM</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -531,12 +531,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1DA</t>
+          <t>APROG</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Prof_B</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -546,7 +546,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CHEM101</t>
+          <t>LEM</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -565,12 +565,12 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1DB</t>
+          <t>CMATE-M</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Prof_C</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -580,7 +580,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ENG101</t>
+          <t>LEM</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -595,16 +595,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1DB</t>
+          <t>FSIAP</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Prof_D</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -614,7 +614,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CS101</t>
+          <t>LEM</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -629,19 +629,2093 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1DC</t>
+          <t>IENG1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Prof_E</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="H6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>FISIC</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>IENG2</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>MATE1</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>MECA1</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>MTMET</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>EMELE</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>MATE2</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>MECA2</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>MTNMT</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>TERMO</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>ELTRO</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>2</v>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>ESTAT</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>MEFLU</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>2</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>MEMAT</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>2</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>PFAB1</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>2</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>AUTO1</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>ORGI1</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>3</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>2</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>ORMAQ</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>3</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>2</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>PFAB2</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>3</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>TRFCA-M</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>3</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>AUTO2</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>3</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>2</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>MFLUX</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>3</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>2</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>MTERM</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>3</v>
+      </c>
+      <c r="C30" t="n">
+        <v>2</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>2</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>ORGI2</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>2</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>ALGAN</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>2</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>DEGER</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>2</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>FSIAP</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>DESET</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>2</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>MATE1</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>2</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>MECA1</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>2</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>2</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>MTMET</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>2</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>MATE2</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>2</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>MECA2</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>2</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>MTNMT</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>2</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>2</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>TERMO</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" t="n">
+        <v>2</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>2</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>ESTAT</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>2</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>MEFLU</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" t="n">
+        <v>2</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>2</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>MEMAT</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" t="n">
+        <v>2</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>2</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>PFAB1</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>3</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>2</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>ORGI1</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>3</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>2</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>ORMAQ</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>3</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>2</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>PFAB2</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>3</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>2</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>TRFCA-M</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>3</v>
+      </c>
+      <c r="C50" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>2</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>MFLUX</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>3</v>
+      </c>
+      <c r="C51" t="n">
+        <v>2</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>2</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>MTERM</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>3</v>
+      </c>
+      <c r="C52" t="n">
+        <v>2</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>2</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>ORGI2</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>2</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>APROG</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>1</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>2</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>CMATE-M</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>1</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>2</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>DEGER</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>2</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>IENG1</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1</v>
+      </c>
+      <c r="C57" t="n">
+        <v>2</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>2</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>DESET</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1</v>
+      </c>
+      <c r="C58" t="n">
+        <v>2</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>2</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>FISIC</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1</v>
+      </c>
+      <c r="C59" t="n">
+        <v>2</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>2</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>IENG2</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>2</v>
+      </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>3</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>CEFAC</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>2</v>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>2</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>EMELE</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>2</v>
+      </c>
+      <c r="C62" t="n">
+        <v>2</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>3</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>ANPRO</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>2</v>
+      </c>
+      <c r="C63" t="n">
+        <v>2</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>2</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>ELTRO</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>3</v>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>2</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>AUTO1</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>3</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>3</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>PROJ1</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>3</v>
+      </c>
+      <c r="C66" t="n">
+        <v>2</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>2</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>AUTO2</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>LEM</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>3</v>
+      </c>
+      <c r="C67" t="n">
+        <v>2</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>PL</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>4</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>PESTM</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>